<commit_message>
DEF and mode shape
partly completed.
</commit_message>
<xml_diff>
--- a/system_cases/Oscillation_July/DEF_IEEE14_case1.xlsx
+++ b/system_cases/Oscillation_July/DEF_IEEE14_case1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Simplus-Grid-Tool\system_cases\Oscillation_July\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED65F1C-A112-412B-9371-821FDFC60019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1FAA1BA-0411-4F7B-A210-52C76F85484E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -1511,8 +1511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34645F5B-1D7A-4323-9AD6-5FF81941CA24}">
   <dimension ref="A1:AW18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3278,8 +3278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EFCB373-2341-40B6-A375-7BA50357479A}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>